<commit_message>
don't double-scale actual data
</commit_message>
<xml_diff>
--- a/in/apr14.xlsx
+++ b/in/apr14.xlsx
@@ -938,7 +938,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1195,6 +1195,10 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1284,7 +1288,7 @@
   <dimension ref="A1:H80"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="79" zoomScaleNormal="79" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="E55" activeCellId="0" sqref="E55"/>
     </sheetView>
@@ -1876,7 +1880,7 @@
       <c r="C54" s="0"/>
       <c r="D54" s="5"/>
       <c r="E54" s="39" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F54" s="13"/>
     </row>
@@ -2001,7 +2005,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="79" zoomScaleNormal="79" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="bottomLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4342,8 +4346,8 @@
       <c r="A10" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B10" s="51"/>
-      <c r="C10" s="51"/>
+      <c r="B10" s="0"/>
+      <c r="C10" s="0"/>
       <c r="D10" s="0"/>
       <c r="E10" s="0"/>
       <c r="F10" s="0"/>
@@ -7942,8 +7946,12 @@
       <c r="A24" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B24" s="0"/>
-      <c r="C24" s="0"/>
+      <c r="B24" s="64" t="n">
+        <v>2150</v>
+      </c>
+      <c r="C24" s="64" t="n">
+        <v>2150</v>
+      </c>
       <c r="D24" s="0"/>
       <c r="E24" s="0"/>
       <c r="F24" s="0"/>
@@ -9033,10 +9041,10 @@
       <c r="A35" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B35" s="64" t="n">
+      <c r="B35" s="65" t="n">
         <v>65.1186367</v>
       </c>
-      <c r="C35" s="64" t="n">
+      <c r="C35" s="65" t="n">
         <v>65.12657</v>
       </c>
     </row>
@@ -9044,10 +9052,10 @@
       <c r="A36" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B36" s="64" t="n">
+      <c r="B36" s="65" t="n">
         <v>-147.432975</v>
       </c>
-      <c r="C36" s="64" t="n">
+      <c r="C36" s="65" t="n">
         <v>-147.496908333</v>
       </c>
     </row>
@@ -9109,11 +9117,11 @@
       <c r="A43" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="B43" s="65" t="n">
+      <c r="B43" s="66" t="n">
         <f aca="false">(0.0016)^2</f>
         <v>2.56E-006</v>
       </c>
-      <c r="C43" s="65" t="n">
+      <c r="C43" s="66" t="n">
         <f aca="false">(0.0016)^2</f>
         <v>2.56E-006</v>
       </c>

</xml_diff>

<commit_message>
INWORK: switching to .h5 data
</commit_message>
<xml_diff>
--- a/in/apr14.xlsx
+++ b/in/apr14.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="984" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sim" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,6 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
             <charset val="1"/>
@@ -100,10 +99,8 @@
       <text>
         <r>
           <rPr>
-            <b val="true"/>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <sz val="10"/>
+            <rFont val="Arial"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -116,7 +113,6 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
             <charset val="1"/>
@@ -130,10 +126,8 @@
       <text>
         <r>
           <rPr>
-            <b val="true"/>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <sz val="10"/>
+            <rFont val="Arial"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -146,10 +140,8 @@
       <text>
         <r>
           <rPr>
-            <b val="true"/>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <sz val="10"/>
+            <rFont val="Arial"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -165,7 +157,6 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
             <charset val="1"/>
@@ -202,7 +193,6 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
             <charset val="1"/>
@@ -217,7 +207,6 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
             <charset val="1"/>
@@ -234,7 +223,6 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
             <charset val="1"/>
@@ -243,7 +231,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A44" authorId="0">
+    <comment ref="A38" authorId="0">
       <text>
         <r>
           <rPr>
@@ -261,7 +249,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="118">
   <si>
     <t>Sim</t>
   </si>
@@ -299,7 +287,7 @@
     <t>ActualDataDir</t>
   </si>
   <si>
-    <t>~/data</t>
+    <t>~/HSTdata/DataField/2013-04-14</t>
   </si>
   <si>
     <t>BG3transFN</t>
@@ -579,21 +567,6 @@
   </si>
   <si>
     <t>savgolOrder</t>
-  </si>
-  <si>
-    <t>xPix</t>
-  </si>
-  <si>
-    <t>yPix</t>
-  </si>
-  <si>
-    <t>xBin</t>
-  </si>
-  <si>
-    <t>yBin</t>
-  </si>
-  <si>
-    <t>nHead16</t>
   </si>
   <si>
     <t>latWGS84</t>
@@ -1287,23 +1260,23 @@
   </sheetPr>
   <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="79" zoomScaleNormal="79" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="36.1071428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.13775510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.70408163265306"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.69897959183673"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="28.5357142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="35.6377551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2000,21 +1973,21 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:IQ45"/>
+  <dimension ref="A1:IQ39"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="79" zoomScaleNormal="79" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="bottomLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="46" width="21.4030612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="46" width="60.9183673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="46" width="48.2448979591837"/>
-    <col collapsed="false" hidden="false" max="251" min="4" style="46" width="10.4132653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="252" style="0" width="10.4132653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="46" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="46" width="60.2040816326531"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="46" width="47.6530612244898"/>
+    <col collapsed="false" hidden="false" max="251" min="4" style="46" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="252" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8981,170 +8954,110 @@
       <c r="A29" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B29" s="0" t="n">
-        <v>512</v>
-      </c>
-      <c r="C29" s="0" t="n">
-        <v>512</v>
+      <c r="B29" s="65" t="n">
+        <v>65.1186367</v>
+      </c>
+      <c r="C29" s="65" t="n">
+        <v>65.12657</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B30" s="0" t="n">
-        <v>512</v>
-      </c>
-      <c r="C30" s="0" t="n">
-        <v>512</v>
+      <c r="B30" s="65" t="n">
+        <v>-147.432975</v>
+      </c>
+      <c r="C30" s="65" t="n">
+        <v>-147.496908333</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B31" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C31" s="0" t="n">
-        <v>1</v>
-      </c>
+      <c r="A31" s="0"/>
+      <c r="B31" s="0"/>
+      <c r="C31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B32" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C32" s="0" t="n">
-        <v>1</v>
+        <v>108</v>
+      </c>
+      <c r="B32" s="4" t="n">
+        <v>77.51</v>
+      </c>
+      <c r="C32" s="4" t="n">
+        <v>77.5</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B33" s="4" t="n">
+        <v>19.92</v>
+      </c>
+      <c r="C33" s="4" t="n">
+        <v>19.9</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B33" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C33" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0"/>
-      <c r="B34" s="0"/>
-      <c r="C34" s="0"/>
+      <c r="B34" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B35" s="65" t="n">
-        <v>65.1186367</v>
-      </c>
-      <c r="C35" s="65" t="n">
-        <v>65.12657</v>
+        <v>112</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B36" s="65" t="n">
-        <v>-147.432975</v>
-      </c>
-      <c r="C36" s="65" t="n">
-        <v>-147.496908333</v>
-      </c>
+      <c r="A36" s="0"/>
+      <c r="B36" s="0"/>
+      <c r="C36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0"/>
-      <c r="B37" s="0"/>
-      <c r="C37" s="0"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B38" s="4" t="n">
-        <v>77.51</v>
-      </c>
-      <c r="C38" s="4" t="n">
-        <v>77.5</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B39" s="4" t="n">
-        <v>19.92</v>
-      </c>
-      <c r="C39" s="4" t="n">
-        <v>19.9</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="4" t="s">
+      <c r="A37" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="B40" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0"/>
-      <c r="B42" s="0"/>
-      <c r="C42" s="0"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="46" t="s">
-        <v>120</v>
-      </c>
-      <c r="B43" s="66" t="n">
+      <c r="B37" s="66" t="n">
         <f aca="false">(0.0016)^2</f>
         <v>2.56E-006</v>
       </c>
-      <c r="C43" s="66" t="n">
+      <c r="C37" s="66" t="n">
         <f aca="false">(0.0016)^2</f>
         <v>2.56E-006</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="46" t="s">
-        <v>121</v>
-      </c>
-      <c r="B44" s="46" t="n">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="B38" s="46" t="n">
         <v>1</v>
       </c>
-      <c r="C44" s="46" t="n">
+      <c r="C38" s="46" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="46" t="s">
-        <v>122</v>
-      </c>
-      <c r="B45" s="46" t="n">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="46" t="s">
+        <v>117</v>
+      </c>
+      <c r="B39" s="46" t="n">
         <v>1</v>
       </c>
-      <c r="C45" s="46" t="n">
+      <c r="C39" s="46" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
gain for real case
</commit_message>
<xml_diff>
--- a/in/apr14.xlsx
+++ b/in/apr14.xlsx
@@ -1199,7 +1199,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="D12" activeCellId="1" sqref="B31:C33 D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1914,7 +1914,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="bottomLeft" activeCell="B31" activeCellId="0" sqref="B31:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -7419,17 +7419,35 @@
       <c r="A31" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="B31" s="60"/>
-      <c r="C31" s="60"/>
+      <c r="B31" s="60" t="n">
+        <f aca="false">(0.0016)^2</f>
+        <v>2.56E-006</v>
+      </c>
+      <c r="C31" s="60" t="n">
+        <f aca="false">(0.0016)^2</f>
+        <v>2.56E-006</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="59" t="s">
         <v>108</v>
       </c>
+      <c r="B32" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" s="46" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="59" t="s">
         <v>109</v>
+      </c>
+      <c r="B33" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="46" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
real data scaling, TODO observe that loading reverses brightness line but not axis
</commit_message>
<xml_diff>
--- a/in/apr14.xlsx
+++ b/in/apr14.xlsx
@@ -871,7 +871,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="60">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1100,10 +1100,6 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1199,20 +1195,19 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E54" activeCellId="0" sqref="E54"/>
+      <selection pane="bottomLeft" activeCell="E55" activeCellId="0" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="33.8826530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="33.4795918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="26.4591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1789,7 +1784,7 @@
       <c r="C54" s="0"/>
       <c r="D54" s="5"/>
       <c r="E54" s="39" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F54" s="13"/>
     </row>
@@ -1914,15 +1909,15 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+      <selection pane="bottomLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="46" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="46" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="251" min="4" style="46" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="252" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="46" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="46" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="251" min="4" style="46" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="252" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6312,8 +6307,12 @@
       <c r="A18" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
+      <c r="B18" s="0" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>1500</v>
+      </c>
       <c r="D18" s="0"/>
       <c r="E18" s="0"/>
       <c r="F18" s="0"/>
@@ -7343,10 +7342,10 @@
       <c r="A23" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B23" s="58" t="n">
+      <c r="B23" s="57" t="n">
         <v>65.1186367</v>
       </c>
-      <c r="C23" s="58" t="n">
+      <c r="C23" s="57" t="n">
         <v>65.12657</v>
       </c>
     </row>
@@ -7354,10 +7353,10 @@
       <c r="A24" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B24" s="58" t="n">
+      <c r="B24" s="57" t="n">
         <v>-147.432975</v>
       </c>
-      <c r="C24" s="58" t="n">
+      <c r="C24" s="57" t="n">
         <v>-147.496908333</v>
       </c>
     </row>
@@ -7416,20 +7415,20 @@
       <c r="C30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="59" t="s">
+      <c r="A31" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="B31" s="60" t="n">
+      <c r="B31" s="59" t="n">
         <f aca="false">(0.0016)^2</f>
         <v>2.56E-006</v>
       </c>
-      <c r="C31" s="60" t="n">
+      <c r="C31" s="59" t="n">
         <f aca="false">(0.0016)^2</f>
         <v>2.56E-006</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="59" t="s">
+      <c r="A32" s="58" t="s">
         <v>108</v>
       </c>
       <c r="B32" s="46" t="n">
@@ -7440,14 +7439,14 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="59" t="s">
+      <c r="A33" s="58" t="s">
         <v>109</v>
       </c>
       <c r="B33" s="46" t="n">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="C33" s="46" t="n">
-        <v>1</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
allow user input, pathlib
</commit_message>
<xml_diff>
--- a/in/apr14.xlsx
+++ b/in/apr14.xlsx
@@ -412,13 +412,13 @@
     <t>reqStartUT</t>
   </si>
   <si>
-    <t>2013-04-14T08:54:22.100Z</t>
+    <t>2013-04-14T08:54:16Z</t>
   </si>
   <si>
     <t>reqStopUT</t>
   </si>
   <si>
-    <t>2013-04-14T08:54:22.400Z</t>
+    <t>2013-04-14T08:54:31Z</t>
   </si>
   <si>
     <t>UseTCz</t>
@@ -1154,7 +1154,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E54" activeCellId="0" sqref="E54"/>
+      <selection pane="bottomLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
allowing real time to propagate, cleaner error trapping
</commit_message>
<xml_diff>
--- a/in/apr14.xlsx
+++ b/in/apr14.xlsx
@@ -223,7 +223,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A18" authorId="0">
+    <comment ref="A16" authorId="0">
       <text>
         <r>
           <rPr>
@@ -236,7 +236,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A27" authorId="0">
+    <comment ref="A25" authorId="0">
       <text>
         <r>
           <rPr>
@@ -254,7 +254,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="102">
   <si>
     <t>Sim</t>
   </si>
@@ -412,13 +412,13 @@
     <t>reqStartUT</t>
   </si>
   <si>
-    <t>2013-04-14T08:54:16Z</t>
+    <t>2013-04-14T08:54:22.100Z</t>
   </si>
   <si>
     <t>reqStopUT</t>
   </si>
   <si>
-    <t>2013-04-14T08:54:31Z</t>
+    <t>2013-04-14T08:54:22.400Z</t>
   </si>
   <si>
     <t>UseTCz</t>
@@ -497,12 +497,6 @@
   </si>
   <si>
     <t>FOVmaxLengthKM</t>
-  </si>
-  <si>
-    <t>noiseLam</t>
-  </si>
-  <si>
-    <t>CCDBias</t>
   </si>
   <si>
     <t>timeShiftSec</t>
@@ -572,11 +566,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="0"/>
-    <numFmt numFmtId="167" formatCode="0.00E+000"/>
+    <numFmt numFmtId="166" formatCode="0.00E+000"/>
   </numFmts>
   <fonts count="17">
     <font>
@@ -850,7 +843,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1039,10 +1032,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1067,7 +1056,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1154,7 +1143,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
+      <selection pane="bottomLeft" activeCell="E54" activeCellId="0" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1596,7 +1585,7 @@
       <c r="B46" s="0"/>
       <c r="C46" s="0"/>
       <c r="D46" s="34" t="n">
-        <v>-3.8</v>
+        <v>-5</v>
       </c>
       <c r="E46" s="35"/>
       <c r="F46" s="0"/>
@@ -1608,7 +1597,7 @@
       <c r="B47" s="0"/>
       <c r="C47" s="0"/>
       <c r="D47" s="34" t="n">
-        <v>7.1</v>
+        <v>10</v>
       </c>
       <c r="E47" s="35"/>
       <c r="F47" s="0"/>
@@ -1787,12 +1776,12 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:IQ28"/>
+  <dimension ref="A1:IQ26"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3359,8 +3348,12 @@
       <c r="A7" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="47"/>
-      <c r="C7" s="47"/>
+      <c r="B7" s="47" t="n">
+        <v>-0.188679245283019</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="D7" s="0"/>
       <c r="E7" s="0"/>
       <c r="F7" s="0"/>
@@ -3614,8 +3607,12 @@
       <c r="A8" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="0"/>
-      <c r="C8" s="0"/>
+      <c r="B8" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>84</v>
+      </c>
       <c r="D8" s="0"/>
       <c r="E8" s="0"/>
       <c r="F8" s="0"/>
@@ -3866,15 +3863,9 @@
       <c r="IQ8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" s="48" t="n">
-        <v>-0.188679245283019</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>0</v>
-      </c>
+      <c r="A9" s="0"/>
+      <c r="B9" s="0"/>
+      <c r="C9" s="49"/>
       <c r="D9" s="0"/>
       <c r="E9" s="0"/>
       <c r="F9" s="0"/>
@@ -4126,13 +4117,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="C10" s="49" t="s">
-        <v>86</v>
+      <c r="B10" s="50" t="n">
+        <v>10</v>
+      </c>
+      <c r="C10" s="51" t="n">
+        <v>1000</v>
       </c>
       <c r="D10" s="0"/>
       <c r="E10" s="0"/>
@@ -4384,9 +4375,15 @@
       <c r="IQ10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0"/>
-      <c r="B11" s="0"/>
-      <c r="C11" s="50"/>
+      <c r="A11" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="50" t="n">
+        <v>35000</v>
+      </c>
+      <c r="C11" s="51" t="n">
+        <v>2500</v>
+      </c>
       <c r="D11" s="0"/>
       <c r="E11" s="0"/>
       <c r="F11" s="0"/>
@@ -4640,11 +4637,11 @@
       <c r="A12" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B12" s="51" t="n">
-        <v>10</v>
-      </c>
-      <c r="C12" s="52" t="n">
-        <v>1000</v>
+      <c r="B12" s="4" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="D12" s="0"/>
       <c r="E12" s="0"/>
@@ -4899,12 +4896,8 @@
       <c r="A13" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B13" s="51" t="n">
-        <v>35000</v>
-      </c>
-      <c r="C13" s="52" t="n">
-        <v>2500</v>
-      </c>
+      <c r="B13" s="0"/>
+      <c r="C13" s="0"/>
       <c r="D13" s="0"/>
       <c r="E13" s="0"/>
       <c r="F13" s="0"/>
@@ -5158,11 +5151,11 @@
       <c r="A14" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B14" s="4" t="n">
-        <v>0.1</v>
+      <c r="B14" s="0" t="n">
+        <v>2000</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>1</v>
+        <v>2000</v>
       </c>
       <c r="D14" s="0"/>
       <c r="E14" s="0"/>
@@ -5414,9 +5407,7 @@
       <c r="IQ14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
-        <v>90</v>
-      </c>
+      <c r="A15" s="0"/>
       <c r="B15" s="0"/>
       <c r="C15" s="0"/>
       <c r="D15" s="0"/>
@@ -5670,17 +5661,17 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B16" s="0" t="n">
-        <v>2200</v>
-      </c>
-      <c r="C16" s="0" t="n">
-        <v>2200</v>
+        <v>90</v>
+      </c>
+      <c r="B16" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="C16" s="5" t="n">
+        <v>15</v>
       </c>
       <c r="D16" s="0"/>
-      <c r="E16" s="0"/>
-      <c r="F16" s="0"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="1"/>
       <c r="G16" s="0"/>
       <c r="H16" s="0"/>
       <c r="I16" s="0"/>
@@ -5928,12 +5919,18 @@
       <c r="IQ16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0"/>
-      <c r="B17" s="0"/>
-      <c r="C17" s="0"/>
+      <c r="A17" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C17" s="5" t="n">
+        <v>2</v>
+      </c>
       <c r="D17" s="0"/>
-      <c r="E17" s="0"/>
-      <c r="F17" s="0"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="1"/>
       <c r="G17" s="0"/>
       <c r="H17" s="0"/>
       <c r="I17" s="0"/>
@@ -6181,609 +6178,91 @@
       <c r="IQ17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B18" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="C18" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="D18" s="0"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="0"/>
-      <c r="H18" s="0"/>
-      <c r="I18" s="0"/>
-      <c r="J18" s="0"/>
-      <c r="K18" s="0"/>
-      <c r="L18" s="0"/>
-      <c r="M18" s="0"/>
-      <c r="N18" s="0"/>
-      <c r="O18" s="0"/>
-      <c r="P18" s="0"/>
-      <c r="Q18" s="0"/>
-      <c r="R18" s="0"/>
-      <c r="S18" s="0"/>
-      <c r="T18" s="0"/>
-      <c r="U18" s="0"/>
-      <c r="V18" s="0"/>
-      <c r="W18" s="0"/>
-      <c r="X18" s="0"/>
-      <c r="Y18" s="0"/>
-      <c r="Z18" s="0"/>
-      <c r="AA18" s="0"/>
-      <c r="AB18" s="0"/>
-      <c r="AC18" s="0"/>
-      <c r="AD18" s="0"/>
-      <c r="AE18" s="0"/>
-      <c r="AF18" s="0"/>
-      <c r="AG18" s="0"/>
-      <c r="AH18" s="0"/>
-      <c r="AI18" s="0"/>
-      <c r="AJ18" s="0"/>
-      <c r="AK18" s="0"/>
-      <c r="AL18" s="0"/>
-      <c r="AM18" s="0"/>
-      <c r="AN18" s="0"/>
-      <c r="AO18" s="0"/>
-      <c r="AP18" s="0"/>
-      <c r="AQ18" s="0"/>
-      <c r="AR18" s="0"/>
-      <c r="AS18" s="0"/>
-      <c r="AT18" s="0"/>
-      <c r="AU18" s="0"/>
-      <c r="AV18" s="0"/>
-      <c r="AW18" s="0"/>
-      <c r="AX18" s="0"/>
-      <c r="AY18" s="0"/>
-      <c r="AZ18" s="0"/>
-      <c r="BA18" s="0"/>
-      <c r="BB18" s="0"/>
-      <c r="BC18" s="0"/>
-      <c r="BD18" s="0"/>
-      <c r="BE18" s="0"/>
-      <c r="BF18" s="0"/>
-      <c r="BG18" s="0"/>
-      <c r="BH18" s="0"/>
-      <c r="BI18" s="0"/>
-      <c r="BJ18" s="0"/>
-      <c r="BK18" s="0"/>
-      <c r="BL18" s="0"/>
-      <c r="BM18" s="0"/>
-      <c r="BN18" s="0"/>
-      <c r="BO18" s="0"/>
-      <c r="BP18" s="0"/>
-      <c r="BQ18" s="0"/>
-      <c r="BR18" s="0"/>
-      <c r="BS18" s="0"/>
-      <c r="BT18" s="0"/>
-      <c r="BU18" s="0"/>
-      <c r="BV18" s="0"/>
-      <c r="BW18" s="0"/>
-      <c r="BX18" s="0"/>
-      <c r="BY18" s="0"/>
-      <c r="BZ18" s="0"/>
-      <c r="CA18" s="0"/>
-      <c r="CB18" s="0"/>
-      <c r="CC18" s="0"/>
-      <c r="CD18" s="0"/>
-      <c r="CE18" s="0"/>
-      <c r="CF18" s="0"/>
-      <c r="CG18" s="0"/>
-      <c r="CH18" s="0"/>
-      <c r="CI18" s="0"/>
-      <c r="CJ18" s="0"/>
-      <c r="CK18" s="0"/>
-      <c r="CL18" s="0"/>
-      <c r="CM18" s="0"/>
-      <c r="CN18" s="0"/>
-      <c r="CO18" s="0"/>
-      <c r="CP18" s="0"/>
-      <c r="CQ18" s="0"/>
-      <c r="CR18" s="0"/>
-      <c r="CS18" s="0"/>
-      <c r="CT18" s="0"/>
-      <c r="CU18" s="0"/>
-      <c r="CV18" s="0"/>
-      <c r="CW18" s="0"/>
-      <c r="CX18" s="0"/>
-      <c r="CY18" s="0"/>
-      <c r="CZ18" s="0"/>
-      <c r="DA18" s="0"/>
-      <c r="DB18" s="0"/>
-      <c r="DC18" s="0"/>
-      <c r="DD18" s="0"/>
-      <c r="DE18" s="0"/>
-      <c r="DF18" s="0"/>
-      <c r="DG18" s="0"/>
-      <c r="DH18" s="0"/>
-      <c r="DI18" s="0"/>
-      <c r="DJ18" s="0"/>
-      <c r="DK18" s="0"/>
-      <c r="DL18" s="0"/>
-      <c r="DM18" s="0"/>
-      <c r="DN18" s="0"/>
-      <c r="DO18" s="0"/>
-      <c r="DP18" s="0"/>
-      <c r="DQ18" s="0"/>
-      <c r="DR18" s="0"/>
-      <c r="DS18" s="0"/>
-      <c r="DT18" s="0"/>
-      <c r="DU18" s="0"/>
-      <c r="DV18" s="0"/>
-      <c r="DW18" s="0"/>
-      <c r="DX18" s="0"/>
-      <c r="DY18" s="0"/>
-      <c r="DZ18" s="0"/>
-      <c r="EA18" s="0"/>
-      <c r="EB18" s="0"/>
-      <c r="EC18" s="0"/>
-      <c r="ED18" s="0"/>
-      <c r="EE18" s="0"/>
-      <c r="EF18" s="0"/>
-      <c r="EG18" s="0"/>
-      <c r="EH18" s="0"/>
-      <c r="EI18" s="0"/>
-      <c r="EJ18" s="0"/>
-      <c r="EK18" s="0"/>
-      <c r="EL18" s="0"/>
-      <c r="EM18" s="0"/>
-      <c r="EN18" s="0"/>
-      <c r="EO18" s="0"/>
-      <c r="EP18" s="0"/>
-      <c r="EQ18" s="0"/>
-      <c r="ER18" s="0"/>
-      <c r="ES18" s="0"/>
-      <c r="ET18" s="0"/>
-      <c r="EU18" s="0"/>
-      <c r="EV18" s="0"/>
-      <c r="EW18" s="0"/>
-      <c r="EX18" s="0"/>
-      <c r="EY18" s="0"/>
-      <c r="EZ18" s="0"/>
-      <c r="FA18" s="0"/>
-      <c r="FB18" s="0"/>
-      <c r="FC18" s="0"/>
-      <c r="FD18" s="0"/>
-      <c r="FE18" s="0"/>
-      <c r="FF18" s="0"/>
-      <c r="FG18" s="0"/>
-      <c r="FH18" s="0"/>
-      <c r="FI18" s="0"/>
-      <c r="FJ18" s="0"/>
-      <c r="FK18" s="0"/>
-      <c r="FL18" s="0"/>
-      <c r="FM18" s="0"/>
-      <c r="FN18" s="0"/>
-      <c r="FO18" s="0"/>
-      <c r="FP18" s="0"/>
-      <c r="FQ18" s="0"/>
-      <c r="FR18" s="0"/>
-      <c r="FS18" s="0"/>
-      <c r="FT18" s="0"/>
-      <c r="FU18" s="0"/>
-      <c r="FV18" s="0"/>
-      <c r="FW18" s="0"/>
-      <c r="FX18" s="0"/>
-      <c r="FY18" s="0"/>
-      <c r="FZ18" s="0"/>
-      <c r="GA18" s="0"/>
-      <c r="GB18" s="0"/>
-      <c r="GC18" s="0"/>
-      <c r="GD18" s="0"/>
-      <c r="GE18" s="0"/>
-      <c r="GF18" s="0"/>
-      <c r="GG18" s="0"/>
-      <c r="GH18" s="0"/>
-      <c r="GI18" s="0"/>
-      <c r="GJ18" s="0"/>
-      <c r="GK18" s="0"/>
-      <c r="GL18" s="0"/>
-      <c r="GM18" s="0"/>
-      <c r="GN18" s="0"/>
-      <c r="GO18" s="0"/>
-      <c r="GP18" s="0"/>
-      <c r="GQ18" s="0"/>
-      <c r="GR18" s="0"/>
-      <c r="GS18" s="0"/>
-      <c r="GT18" s="0"/>
-      <c r="GU18" s="0"/>
-      <c r="GV18" s="0"/>
-      <c r="GW18" s="0"/>
-      <c r="GX18" s="0"/>
-      <c r="GY18" s="0"/>
-      <c r="GZ18" s="0"/>
-      <c r="HA18" s="0"/>
-      <c r="HB18" s="0"/>
-      <c r="HC18" s="0"/>
-      <c r="HD18" s="0"/>
-      <c r="HE18" s="0"/>
-      <c r="HF18" s="0"/>
-      <c r="HG18" s="0"/>
-      <c r="HH18" s="0"/>
-      <c r="HI18" s="0"/>
-      <c r="HJ18" s="0"/>
-      <c r="HK18" s="0"/>
-      <c r="HL18" s="0"/>
-      <c r="HM18" s="0"/>
-      <c r="HN18" s="0"/>
-      <c r="HO18" s="0"/>
-      <c r="HP18" s="0"/>
-      <c r="HQ18" s="0"/>
-      <c r="HR18" s="0"/>
-      <c r="HS18" s="0"/>
-      <c r="HT18" s="0"/>
-      <c r="HU18" s="0"/>
-      <c r="HV18" s="0"/>
-      <c r="HW18" s="0"/>
-      <c r="HX18" s="0"/>
-      <c r="HY18" s="0"/>
-      <c r="HZ18" s="0"/>
-      <c r="IA18" s="0"/>
-      <c r="IB18" s="0"/>
-      <c r="IC18" s="0"/>
-      <c r="ID18" s="0"/>
-      <c r="IE18" s="0"/>
-      <c r="IF18" s="0"/>
-      <c r="IG18" s="0"/>
-      <c r="IH18" s="0"/>
-      <c r="II18" s="0"/>
-      <c r="IJ18" s="0"/>
-      <c r="IK18" s="0"/>
-      <c r="IL18" s="0"/>
-      <c r="IM18" s="0"/>
-      <c r="IN18" s="0"/>
-      <c r="IO18" s="0"/>
-      <c r="IP18" s="0"/>
-      <c r="IQ18" s="0"/>
+      <c r="A18" s="0"/>
+      <c r="B18" s="0"/>
+      <c r="C18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="4" t="n">
+        <v>77.51</v>
+      </c>
+      <c r="C19" s="4" t="n">
+        <v>77.5</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B19" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C19" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="D19" s="0"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="0"/>
-      <c r="H19" s="0"/>
-      <c r="I19" s="0"/>
-      <c r="J19" s="0"/>
-      <c r="K19" s="0"/>
-      <c r="L19" s="0"/>
-      <c r="M19" s="0"/>
-      <c r="N19" s="0"/>
-      <c r="O19" s="0"/>
-      <c r="P19" s="0"/>
-      <c r="Q19" s="0"/>
-      <c r="R19" s="0"/>
-      <c r="S19" s="0"/>
-      <c r="T19" s="0"/>
-      <c r="U19" s="0"/>
-      <c r="V19" s="0"/>
-      <c r="W19" s="0"/>
-      <c r="X19" s="0"/>
-      <c r="Y19" s="0"/>
-      <c r="Z19" s="0"/>
-      <c r="AA19" s="0"/>
-      <c r="AB19" s="0"/>
-      <c r="AC19" s="0"/>
-      <c r="AD19" s="0"/>
-      <c r="AE19" s="0"/>
-      <c r="AF19" s="0"/>
-      <c r="AG19" s="0"/>
-      <c r="AH19" s="0"/>
-      <c r="AI19" s="0"/>
-      <c r="AJ19" s="0"/>
-      <c r="AK19" s="0"/>
-      <c r="AL19" s="0"/>
-      <c r="AM19" s="0"/>
-      <c r="AN19" s="0"/>
-      <c r="AO19" s="0"/>
-      <c r="AP19" s="0"/>
-      <c r="AQ19" s="0"/>
-      <c r="AR19" s="0"/>
-      <c r="AS19" s="0"/>
-      <c r="AT19" s="0"/>
-      <c r="AU19" s="0"/>
-      <c r="AV19" s="0"/>
-      <c r="AW19" s="0"/>
-      <c r="AX19" s="0"/>
-      <c r="AY19" s="0"/>
-      <c r="AZ19" s="0"/>
-      <c r="BA19" s="0"/>
-      <c r="BB19" s="0"/>
-      <c r="BC19" s="0"/>
-      <c r="BD19" s="0"/>
-      <c r="BE19" s="0"/>
-      <c r="BF19" s="0"/>
-      <c r="BG19" s="0"/>
-      <c r="BH19" s="0"/>
-      <c r="BI19" s="0"/>
-      <c r="BJ19" s="0"/>
-      <c r="BK19" s="0"/>
-      <c r="BL19" s="0"/>
-      <c r="BM19" s="0"/>
-      <c r="BN19" s="0"/>
-      <c r="BO19" s="0"/>
-      <c r="BP19" s="0"/>
-      <c r="BQ19" s="0"/>
-      <c r="BR19" s="0"/>
-      <c r="BS19" s="0"/>
-      <c r="BT19" s="0"/>
-      <c r="BU19" s="0"/>
-      <c r="BV19" s="0"/>
-      <c r="BW19" s="0"/>
-      <c r="BX19" s="0"/>
-      <c r="BY19" s="0"/>
-      <c r="BZ19" s="0"/>
-      <c r="CA19" s="0"/>
-      <c r="CB19" s="0"/>
-      <c r="CC19" s="0"/>
-      <c r="CD19" s="0"/>
-      <c r="CE19" s="0"/>
-      <c r="CF19" s="0"/>
-      <c r="CG19" s="0"/>
-      <c r="CH19" s="0"/>
-      <c r="CI19" s="0"/>
-      <c r="CJ19" s="0"/>
-      <c r="CK19" s="0"/>
-      <c r="CL19" s="0"/>
-      <c r="CM19" s="0"/>
-      <c r="CN19" s="0"/>
-      <c r="CO19" s="0"/>
-      <c r="CP19" s="0"/>
-      <c r="CQ19" s="0"/>
-      <c r="CR19" s="0"/>
-      <c r="CS19" s="0"/>
-      <c r="CT19" s="0"/>
-      <c r="CU19" s="0"/>
-      <c r="CV19" s="0"/>
-      <c r="CW19" s="0"/>
-      <c r="CX19" s="0"/>
-      <c r="CY19" s="0"/>
-      <c r="CZ19" s="0"/>
-      <c r="DA19" s="0"/>
-      <c r="DB19" s="0"/>
-      <c r="DC19" s="0"/>
-      <c r="DD19" s="0"/>
-      <c r="DE19" s="0"/>
-      <c r="DF19" s="0"/>
-      <c r="DG19" s="0"/>
-      <c r="DH19" s="0"/>
-      <c r="DI19" s="0"/>
-      <c r="DJ19" s="0"/>
-      <c r="DK19" s="0"/>
-      <c r="DL19" s="0"/>
-      <c r="DM19" s="0"/>
-      <c r="DN19" s="0"/>
-      <c r="DO19" s="0"/>
-      <c r="DP19" s="0"/>
-      <c r="DQ19" s="0"/>
-      <c r="DR19" s="0"/>
-      <c r="DS19" s="0"/>
-      <c r="DT19" s="0"/>
-      <c r="DU19" s="0"/>
-      <c r="DV19" s="0"/>
-      <c r="DW19" s="0"/>
-      <c r="DX19" s="0"/>
-      <c r="DY19" s="0"/>
-      <c r="DZ19" s="0"/>
-      <c r="EA19" s="0"/>
-      <c r="EB19" s="0"/>
-      <c r="EC19" s="0"/>
-      <c r="ED19" s="0"/>
-      <c r="EE19" s="0"/>
-      <c r="EF19" s="0"/>
-      <c r="EG19" s="0"/>
-      <c r="EH19" s="0"/>
-      <c r="EI19" s="0"/>
-      <c r="EJ19" s="0"/>
-      <c r="EK19" s="0"/>
-      <c r="EL19" s="0"/>
-      <c r="EM19" s="0"/>
-      <c r="EN19" s="0"/>
-      <c r="EO19" s="0"/>
-      <c r="EP19" s="0"/>
-      <c r="EQ19" s="0"/>
-      <c r="ER19" s="0"/>
-      <c r="ES19" s="0"/>
-      <c r="ET19" s="0"/>
-      <c r="EU19" s="0"/>
-      <c r="EV19" s="0"/>
-      <c r="EW19" s="0"/>
-      <c r="EX19" s="0"/>
-      <c r="EY19" s="0"/>
-      <c r="EZ19" s="0"/>
-      <c r="FA19" s="0"/>
-      <c r="FB19" s="0"/>
-      <c r="FC19" s="0"/>
-      <c r="FD19" s="0"/>
-      <c r="FE19" s="0"/>
-      <c r="FF19" s="0"/>
-      <c r="FG19" s="0"/>
-      <c r="FH19" s="0"/>
-      <c r="FI19" s="0"/>
-      <c r="FJ19" s="0"/>
-      <c r="FK19" s="0"/>
-      <c r="FL19" s="0"/>
-      <c r="FM19" s="0"/>
-      <c r="FN19" s="0"/>
-      <c r="FO19" s="0"/>
-      <c r="FP19" s="0"/>
-      <c r="FQ19" s="0"/>
-      <c r="FR19" s="0"/>
-      <c r="FS19" s="0"/>
-      <c r="FT19" s="0"/>
-      <c r="FU19" s="0"/>
-      <c r="FV19" s="0"/>
-      <c r="FW19" s="0"/>
-      <c r="FX19" s="0"/>
-      <c r="FY19" s="0"/>
-      <c r="FZ19" s="0"/>
-      <c r="GA19" s="0"/>
-      <c r="GB19" s="0"/>
-      <c r="GC19" s="0"/>
-      <c r="GD19" s="0"/>
-      <c r="GE19" s="0"/>
-      <c r="GF19" s="0"/>
-      <c r="GG19" s="0"/>
-      <c r="GH19" s="0"/>
-      <c r="GI19" s="0"/>
-      <c r="GJ19" s="0"/>
-      <c r="GK19" s="0"/>
-      <c r="GL19" s="0"/>
-      <c r="GM19" s="0"/>
-      <c r="GN19" s="0"/>
-      <c r="GO19" s="0"/>
-      <c r="GP19" s="0"/>
-      <c r="GQ19" s="0"/>
-      <c r="GR19" s="0"/>
-      <c r="GS19" s="0"/>
-      <c r="GT19" s="0"/>
-      <c r="GU19" s="0"/>
-      <c r="GV19" s="0"/>
-      <c r="GW19" s="0"/>
-      <c r="GX19" s="0"/>
-      <c r="GY19" s="0"/>
-      <c r="GZ19" s="0"/>
-      <c r="HA19" s="0"/>
-      <c r="HB19" s="0"/>
-      <c r="HC19" s="0"/>
-      <c r="HD19" s="0"/>
-      <c r="HE19" s="0"/>
-      <c r="HF19" s="0"/>
-      <c r="HG19" s="0"/>
-      <c r="HH19" s="0"/>
-      <c r="HI19" s="0"/>
-      <c r="HJ19" s="0"/>
-      <c r="HK19" s="0"/>
-      <c r="HL19" s="0"/>
-      <c r="HM19" s="0"/>
-      <c r="HN19" s="0"/>
-      <c r="HO19" s="0"/>
-      <c r="HP19" s="0"/>
-      <c r="HQ19" s="0"/>
-      <c r="HR19" s="0"/>
-      <c r="HS19" s="0"/>
-      <c r="HT19" s="0"/>
-      <c r="HU19" s="0"/>
-      <c r="HV19" s="0"/>
-      <c r="HW19" s="0"/>
-      <c r="HX19" s="0"/>
-      <c r="HY19" s="0"/>
-      <c r="HZ19" s="0"/>
-      <c r="IA19" s="0"/>
-      <c r="IB19" s="0"/>
-      <c r="IC19" s="0"/>
-      <c r="ID19" s="0"/>
-      <c r="IE19" s="0"/>
-      <c r="IF19" s="0"/>
-      <c r="IG19" s="0"/>
-      <c r="IH19" s="0"/>
-      <c r="II19" s="0"/>
-      <c r="IJ19" s="0"/>
-      <c r="IK19" s="0"/>
-      <c r="IL19" s="0"/>
-      <c r="IM19" s="0"/>
-      <c r="IN19" s="0"/>
-      <c r="IO19" s="0"/>
-      <c r="IP19" s="0"/>
-      <c r="IQ19" s="0"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0"/>
-      <c r="B20" s="0"/>
-      <c r="C20" s="0"/>
+      <c r="B20" s="4" t="n">
+        <v>19.92</v>
+      </c>
+      <c r="C20" s="4" t="n">
+        <v>19.9</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B21" s="4" t="n">
-        <v>77.51</v>
-      </c>
-      <c r="C21" s="4" t="n">
-        <v>77.5</v>
+      <c r="B21" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B22" s="4" t="n">
-        <v>19.92</v>
-      </c>
-      <c r="C22" s="4" t="n">
-        <v>19.9</v>
+        <v>96</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>97</v>
-      </c>
+      <c r="A23" s="0"/>
+      <c r="B23" s="0"/>
+      <c r="C23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B24" s="4" t="s">
+      <c r="A24" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0"/>
-      <c r="B25" s="0"/>
-      <c r="C25" s="0"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="53" t="s">
-        <v>101</v>
-      </c>
-      <c r="B26" s="54" t="n">
+      <c r="B24" s="53" t="n">
         <f aca="false">(0.0016)^2</f>
         <v>2.56E-006</v>
       </c>
-      <c r="C26" s="54" t="n">
+      <c r="C24" s="53" t="n">
         <f aca="false">(0.0016)^2</f>
         <v>2.56E-006</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="53" t="s">
-        <v>102</v>
-      </c>
-      <c r="B27" s="42" t="n">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="42" t="n">
         <v>1</v>
       </c>
-      <c r="C27" s="42" t="n">
+      <c r="C25" s="42" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="53" t="s">
-        <v>103</v>
-      </c>
-      <c r="B28" s="42" t="n">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="52" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" s="42" t="n">
         <v>200</v>
       </c>
-      <c r="C28" s="42" t="n">
+      <c r="C26" s="42" t="n">
         <v>200</v>
       </c>
     </row>

</xml_diff>

<commit_message>
proper formatting of time to string
</commit_message>
<xml_diff>
--- a/in/apr14.xlsx
+++ b/in/apr14.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sim" sheetId="1" state="visible" r:id="rId2"/>
@@ -1140,21 +1140,20 @@
   </sheetPr>
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E54" activeCellId="0" sqref="E54"/>
+      <selection pane="bottomLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.9132653061224"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.20918367346939"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="24.3010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1778,18 +1777,18 @@
   </sheetPr>
   <dimension ref="A1:IQ26"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="42" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="42" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="251" min="4" style="42" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="252" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="42" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="42" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="251" min="4" style="42" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="252" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4638,7 +4637,8 @@
         <v>87</v>
       </c>
       <c r="B12" s="4" t="n">
-        <v>0.1</v>
+        <f aca="false">1/9</f>
+        <v>0.111111111111111</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>1</v>
@@ -5152,10 +5152,10 @@
         <v>89</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="D14" s="0"/>
       <c r="E14" s="0"/>

</xml_diff>